<commit_message>
Add RACI matrix and management docx spreadsheet to the lab directory
</commit_message>
<xml_diff>
--- a/lab/composant.xlsx
+++ b/lab/composant.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\debian\repo\GreenMind\lab\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4672F90-38D0-4560-8E0B-B04293A93E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,115 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Unité centrale &amp; calcul</t>
+  </si>
+  <si>
+    <t>Vision &amp; IA</t>
+  </si>
+  <si>
+    <t>Capteurs</t>
+  </si>
+  <si>
+    <t>Actionneurs</t>
+  </si>
+  <si>
+    <t>Électronique &amp; alimentation</t>
+  </si>
+  <si>
+    <t>Structure et robotique</t>
+  </si>
+  <si>
+    <t>ESP32 DevKit v1
+🔗 Gotronic.fr
+🎯 Rôle : acquisition capteurs + pilotage actionneurs (pompe, LED, ventilateurs, servo).
+✅ Choix : Wi-Fi intégré, faible coût, bonne réactivité pour temps réel.</t>
+  </si>
+  <si>
+    <t>Caméra Raspberry Pi (HQ Camera ou Camera Module V2)
+🔗 Kubii.fr
+🎯 Rôle : vision IA (analyse des plantes, détection maladies, suivi croissance).
+✅ Choix : compatible Pi, bonne résolution pour entraînement modèles vision.</t>
+  </si>
+  <si>
+    <t>Capteur température / humidité air DHT22 (ou SHT31 pour plus de précision)
+🔗 Gotronic.fr
+🎯 Rôle : surveiller climat interne de la serre.
+✅ Choix : simple, fiable, facile à interfacer avec ESP32.</t>
+  </si>
+  <si>
+    <t>Capteur humidité du sol capacitif
+🔗 Amazon.fr
+🎯 Rôle : détecter si le sol est sec → déclencher pompe.
+✅ Choix : capacitif = plus durable (résistif s’oxyde).</t>
+  </si>
+  <si>
+    <t>Capteur luminosité (TSL2561 ou BH1750)
+🔗 Gotronic.fr
+🎯 Rôle : mesurer intensité lumineuse → ajuster LEDs.
+✅ Choix : mesure en lux, facile via I2C.</t>
+  </si>
+  <si>
+    <t>Pompe à eau + tuyaux + électrovanne 12V
+🔗 Conrad.fr
+🎯 Rôle : arroser automatiquement les plants.
+✅ Choix : 12V, débit adapté aux mini-serres.</t>
+  </si>
+  <si>
+    <t>Servomoteur SG90 / MG996R
+🔗 Gotronic.fr
+🎯 Rôle : bras robotique pour semer les graines / ouvrir la porte.
+✅ Choix : couple correct, facile à piloter via ESP32.</t>
+  </si>
+  <si>
+    <t>Ventilateurs 5V/12V (type PC)
+🔗 Amazon.fr
+🎯 Rôle : ventilation serre pour réguler chaleur et humidité.
+✅ Choix : économiques, silencieux, facile à contrôler par relais/MOSFET.</t>
+  </si>
+  <si>
+    <t>LED horticoles (rouge/bleu ou full spectrum)
+🔗 Amazon.fr
+🎯 Rôle : fournir lumière adaptée à la photosynthèse.
+✅ Choix : spectre optimisé pour plantes.</t>
+  </si>
+  <si>
+    <t>Relais ou MOSFET drivers
+🔗 Gotronic.fr
+🎯 Rôle : commander pompe, ventilateurs, LEDs à partir de l’ESP32.
+✅ Choix : indispensable pour isoler logique (3.3V) et puissance (12V).</t>
+  </si>
+  <si>
+    <t>Alimentation 12V 5A (serre) + convertisseur step-down (buck 12V→5V/3.3V)
+🔗 Gotronic.fr
+🎯 Rôle : alimenter pompe, ventilateurs, et réguler pour ESP32 + Raspberry.
+✅ Choix : un seul bloc d’alimentation, distribution via convertisseurs.</t>
+  </si>
+  <si>
+    <t>Mini-serre de table / bac de culture
+🔗 Amazon.fr
+🎯 Rôle : cadre physique pour intégrer capteurs + actionneurs.</t>
+  </si>
+  <si>
+    <t>Bras robotique DIY (type 4-6 axes en kit)
+🔗 Aliexpress.com
+🎯 Rôle : automatiser plantation de graines.
+✅ Choix : peu coûteux, pilotable par servos + ESP32.</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 3 (ou 4 si possible)
+🔗 Kubii.fr
+🎯 Rôle : héberge l’IA (vision avec caméra), serveur web (AppWeb), orchestrateur MQTT.
+✅ Choix :</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +140,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +177,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +492,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="45" customWidth="1"/>
+    <col min="4" max="4" width="52.33203125" customWidth="1"/>
+    <col min="5" max="5" width="50.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="175.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="211.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="208.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="79.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:6" ht="52.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:6" ht="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add composant spreadsheet to the lab directory
</commit_message>
<xml_diff>
--- a/lab/composant.xlsx
+++ b/lab/composant.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\debian\repo\GreenMind\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4672F90-38D0-4560-8E0B-B04293A93E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691C5B0F-C8A7-4D61-8F0F-50194368502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="bras robotisés" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Unité centrale &amp; calcul</t>
   </si>
@@ -126,13 +127,106 @@
 🔗 Kubii.fr
 🎯 Rôle : héberge l’IA (vision avec caméra), serveur web (AppWeb), orchestrateur MQTT.
 ✅ Choix :</t>
+  </si>
+  <si>
+    <t>Critère</t>
+  </si>
+  <si>
+    <t>Valeur recommandée</t>
+  </si>
+  <si>
+    <t>Pourquoi c’est important</t>
+  </si>
+  <si>
+    <t>Nombre d’axes (degrés de liberté)</t>
+  </si>
+  <si>
+    <t>minimum 3–4 axes</t>
+  </si>
+  <si>
+    <t>suffisant pour poser une graine, plus pour des mouvements complexes</t>
+  </si>
+  <si>
+    <t>Portée / reach</t>
+  </si>
+  <si>
+    <t>~10–30 cm (ou plus selon taille serre)</t>
+  </si>
+  <si>
+    <t>pour atteindre différentes zones de plantation</t>
+  </si>
+  <si>
+    <t>Charge utile / payload</t>
+  </si>
+  <si>
+    <t>50–200 g (selon grain + mécanisme)</t>
+  </si>
+  <si>
+    <t>pour supporter le poids du mécanisme de semis</t>
+  </si>
+  <si>
+    <t>Précision / répétabilité</t>
+  </si>
+  <si>
+    <t>&lt; ±1 cm (voire &lt; ±5 mm)</t>
+  </si>
+  <si>
+    <t>pour positionner les graines correctement</t>
+  </si>
+  <si>
+    <t>Interface / contrôle</t>
+  </si>
+  <si>
+    <t>UART, PWM, I2C, librairie / API</t>
+  </si>
+  <si>
+    <t>pour l’intégrer avec ESP32 / Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Matériau / robustesse</t>
+  </si>
+  <si>
+    <t>métal, aluminium, plastique renforcé</t>
+  </si>
+  <si>
+    <t>résister à l’humidité ou contraintes mécaniques</t>
+  </si>
+  <si>
+    <t>Support &amp; documentation</t>
+  </si>
+  <si>
+    <t>code d’exemple, schémas, tutoriels</t>
+  </si>
+  <si>
+    <t>facilite l’intégration dans ton projet</t>
+  </si>
+  <si>
+    <t>Coût &amp; disponibilité</t>
+  </si>
+  <si>
+    <t>budget faible / intermédiaire</t>
+  </si>
+  <si>
+    <t>pour ton prototype, pas besoin de bras industriel complet</t>
+  </si>
+  <si>
+    <t>Lien</t>
+  </si>
+  <si>
+    <t>https://www.lextronic.fr/bras-robotique-mearm-classic-maker-kit-63665.html</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/robotique-m%C3%A9canique-Raspberry-%C3%A9tudiants-Bricolage/dp/B08P4WQ82H/ref=sr_1_24?crid=2NYO0WA18RQYS&amp;dib=eyJ2IjoiMSJ9.5ENYusLGTOI7QWPhaq_mQmjmVKKSvUf24MaU_5X2Hv5ZxAWQ1ozNTjWIIwEys10Ba1AvODQwj-omkEoK8AFJb4M0_Y4wHypVprQgj2Vd5aNDUFE-kL_8mQXsDqFWqYf_aTLwWqCrisASQn2Zspo9vGxNxAE9YnsEo7ZJc5FXjk1-D1TI2zceO6-sGbKt7u1SZwbV707TG-uIMdRPgp9dk6KFcmeBthiooos8av9JVtHupYD_hd8mtc39MgVqRfUNc9NOF_aLElb04PEWYPLXXgDCW0uFyvGRXsGaye9-e_w.TVI2qY_OnTWRlt5ADNceLDMtlvh9nPRF-AJGI-tjUAg&amp;dib_tag=se&amp;keywords=bras+robotique&amp;qid=1759327465&amp;sprefix=bras+r%2Caps%2C875&amp;sr=8-24</t>
+  </si>
+  <si>
+    <t>https://www.amazon.fr/Tatiy-Programmation-Servomoteurs-lenseignement-Universitaire/dp/B0B4VKYQ6S/ref=sr_1_29?crid=2NYO0WA18RQYS&amp;dib=eyJ2IjoiMSJ9.5ENYusLGTOI7QWPhaq_mQmjmVKKSvUf24MaU_5X2Hv5ZxAWQ1ozNTjWIIwEys10Ba1AvODQwj-omkEoK8AFJb4M0_Y4wHypVprQgj2Vd5aNDUFE-kL_8mQXsDqFWqYf_aTLwWqCrisASQn2Zspo9vGxNxAE9YnsEo7ZJc5FXjk1-D1TI2zceO6-sGbKt7u1SZwbV707TG-uIMdRPgp9dk6KFcmeBthiooos8av9JVtHupYD_hd8mtc39MgVqRfUNc9NOF_aLElb04PEWYPLXXgDCW0uFyvGRXsGaye9-e_w.TVI2qY_OnTWRlt5ADNceLDMtlvh9nPRF-AJGI-tjUAg&amp;dib_tag=se&amp;keywords=bras+robotique&amp;qid=1759327465&amp;sprefix=bras+r%2Caps%2C875&amp;sr=8-29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +238,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,28 +295,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -495,100 +609,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="58" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="4" width="52.33203125" customWidth="1"/>
-    <col min="5" max="5" width="50.33203125" customWidth="1"/>
-    <col min="6" max="6" width="34.88671875" customWidth="1"/>
+    <col min="1" max="1" width="51.5546875" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" customWidth="1"/>
+    <col min="3" max="3" width="57.33203125" customWidth="1"/>
+    <col min="4" max="4" width="57.44140625" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
+    <col min="6" max="6" width="53.33203125" customWidth="1"/>
     <col min="7" max="7" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="175.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="211.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="208.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="3" t="s">
+    <row r="4" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="187.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:6" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="79.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -599,4 +713,140 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201B0624-01AD-4B82-ADAD-22D5C40CFB72}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
+    <col min="4" max="4" width="111.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7533AB4E-64FF-46AC-BFCD-F24B78523044}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update composants xlsx file
</commit_message>
<xml_diff>
--- a/lab/composant.xlsx
+++ b/lab/composant.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\debian\repo\GreenMind\lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691C5B0F-C8A7-4D61-8F0F-50194368502B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F106E108-0D26-4297-B707-E054CEC82137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="bras robotisés" sheetId="2" r:id="rId2"/>
+    <sheet name="IA" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Unité centrale &amp; calcul</t>
   </si>
@@ -220,6 +221,31 @@
   </si>
   <si>
     <t>https://www.amazon.fr/Tatiy-Programmation-Servomoteurs-lenseignement-Universitaire/dp/B0B4VKYQ6S/ref=sr_1_29?crid=2NYO0WA18RQYS&amp;dib=eyJ2IjoiMSJ9.5ENYusLGTOI7QWPhaq_mQmjmVKKSvUf24MaU_5X2Hv5ZxAWQ1ozNTjWIIwEys10Ba1AvODQwj-omkEoK8AFJb4M0_Y4wHypVprQgj2Vd5aNDUFE-kL_8mQXsDqFWqYf_aTLwWqCrisASQn2Zspo9vGxNxAE9YnsEo7ZJc5FXjk1-D1TI2zceO6-sGbKt7u1SZwbV707TG-uIMdRPgp9dk6KFcmeBthiooos8av9JVtHupYD_hd8mtc39MgVqRfUNc9NOF_aLElb04PEWYPLXXgDCW0uFyvGRXsGaye9-e_w.TVI2qY_OnTWRlt5ADNceLDMtlvh9nPRF-AJGI-tjUAg&amp;dib_tag=se&amp;keywords=bras+robotique&amp;qid=1759327465&amp;sprefix=bras+r%2Caps%2C875&amp;sr=8-29</t>
+  </si>
+  <si>
+    <t>https://scikit-learn.org/stable/install.html</t>
+  </si>
+  <si>
+    <t>Pour la recommandation de plantes
+k-Nearest Neighbors (kNN) (Scikit-learn) :
+Tu stockes une base de données de plantes (tomates, salades, etc.) avec leurs conditions optimales.
+Le modèle compare les conditions actuelles avec celles en base.
+✅ Simple à coder, rapide, idéal pour la Pi.</t>
+  </si>
+  <si>
+    <t>https://scikit-learn.org/stable/modules/generated/sklearn.neighbors.KNeighborsClassifier.html</t>
+  </si>
+  <si>
+    <t>(OpenCV/YOLO) pour détecter où planter</t>
+  </si>
+  <si>
+    <t>Pipeline possible :
+L’utilisateur dit : “J’ai des graines de tomates.”
+Le système :
+Vérifie si les conditions conviennent (via kNN ou règles de similarité).
+Répond : “Oui, vous pouvez planter des tomates.”
+Si oui → la Raspberry Pi envoie un ordre au bras robotique (ESP32) pour exécuter la séquence de plantation.
+Ici pas besoin de ML, juste un script de mouvements servo.</t>
   </si>
 </sst>
 </file>
@@ -299,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -609,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="58" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A3" zoomScale="58" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="190.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
@@ -664,11 +693,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
@@ -682,7 +713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="169.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="8" t="s">
@@ -694,7 +725,7 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="148.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -719,7 +750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201B0624-01AD-4B82-ADAD-22D5C40CFB72}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -745,7 +776,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
@@ -759,7 +790,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
@@ -773,7 +804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>29</v>
       </c>
@@ -787,7 +818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -798,7 +829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
@@ -809,7 +840,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
@@ -820,7 +851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>41</v>
       </c>
@@ -831,7 +862,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
@@ -849,4 +880,46 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C019BC-E91F-4F9C-8E52-10EB4FD93CCB}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{A5A0A582-4FC9-44D7-AA4F-A1734821574B}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{A879C2B0-22B8-45CD-9E0E-83EC3D480A92}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>